<commit_message>
analyze a second run
</commit_message>
<xml_diff>
--- a/examples/test-runs/phase1-xlsx/run-20250128-181630.xlsx
+++ b/examples/test-runs/phase1-xlsx/run-20250128-181630.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="333">
   <si>
     <t xml:space="preserve">timestamp</t>
   </si>
@@ -2508,6 +2508,9 @@
   </si>
   <si>
     <t xml:space="preserve">CertEnroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.asp file</t>
   </si>
   <si>
     <t xml:space="preserve">ESC</t>
@@ -5659,7 +5662,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5681,12 +5684,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5744,7 +5741,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5943,9 +5940,9 @@
   <dimension ref="A1:AM38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AA37" activeCellId="0" sqref="AA37"/>
+      <selection pane="bottomLeft" activeCell="AD25" activeCellId="0" sqref="AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5955,11 +5952,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.32"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="25" min="18" style="1" width="8.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="30.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="91.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="91.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="17.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="15.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="17.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="15.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6831,7 +6828,6 @@
       <c r="AB9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AG9" s="1"/>
       <c r="AI9" s="1" t="s">
         <v>71</v>
       </c>
@@ -7475,7 +7471,7 @@
         <v>144</v>
       </c>
       <c r="AF15" s="1"/>
-      <c r="AI15" s="0" t="s">
+      <c r="AI15" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AJ15" s="1" t="s">
@@ -7578,10 +7574,10 @@
       <c r="AB16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC16" s="0" t="s">
+      <c r="AC16" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AD16" s="0" t="s">
+      <c r="AD16" s="1" t="s">
         <v>155</v>
       </c>
       <c r="AF16" s="1"/>
@@ -7688,7 +7684,7 @@
       <c r="AB17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC17" s="0" t="s">
+      <c r="AC17" s="1" t="s">
         <v>162</v>
       </c>
       <c r="AF17" s="1"/>
@@ -7792,13 +7788,13 @@
       <c r="AA18" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="AD18" s="0" t="s">
+      <c r="AD18" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AI18" s="0" t="s">
+      <c r="AI18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ18" s="0" t="s">
+      <c r="AJ18" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AK18" s="1" t="b">
@@ -7895,16 +7891,16 @@
       <c r="AA19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AC19" s="0" t="s">
+      <c r="AC19" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AE19" s="0" t="s">
+      <c r="AE19" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AI19" s="0" t="s">
+      <c r="AI19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ19" s="0" t="s">
+      <c r="AJ19" s="1" t="s">
         <v>120</v>
       </c>
       <c r="AK19" s="1" t="b">
@@ -8001,16 +7997,16 @@
       <c r="AA20" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AF20" s="0" t="s">
+      <c r="AF20" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AG20" s="0" t="n">
+      <c r="AG20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI20" s="0" t="s">
+      <c r="AI20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ20" s="0" t="s">
+      <c r="AJ20" s="1" t="s">
         <v>82</v>
       </c>
       <c r="AK20" s="1" t="b">
@@ -8107,19 +8103,19 @@
       <c r="AA21" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AF21" s="0" t="s">
+      <c r="AF21" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AG21" s="0" t="n">
+      <c r="AG21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AH21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI21" s="0" t="s">
+      <c r="AI21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ21" s="0" t="s">
+      <c r="AJ21" s="1" t="s">
         <v>82</v>
       </c>
       <c r="AK21" s="1" t="b">
@@ -8216,10 +8212,10 @@
       <c r="AA22" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="AI22" s="0" t="s">
+      <c r="AI22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ22" s="0" t="s">
+      <c r="AJ22" s="1" t="s">
         <v>136</v>
       </c>
       <c r="AK22" s="1" t="b">
@@ -8316,16 +8312,16 @@
       <c r="AA23" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="AC23" s="0" t="s">
+      <c r="AC23" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AE23" s="0" t="s">
+      <c r="AE23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="AI23" s="0" t="s">
+      <c r="AI23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ23" s="0" t="s">
+      <c r="AJ23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AK23" s="1" t="b">
@@ -8422,16 +8418,19 @@
       <c r="AA24" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="AC24" s="0" t="s">
+      <c r="AC24" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AE24" s="0" t="s">
+      <c r="AD24" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="AI24" s="0" t="s">
+      <c r="AE24" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AI24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ24" s="0" t="s">
+      <c r="AJ24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AK24" s="1" t="b">
@@ -8442,12 +8441,12 @@
         <v>71</v>
       </c>
       <c r="AM24" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>31</v>
@@ -8468,10 +8467,10 @@
         <v>0</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>31</v>
@@ -8492,10 +8491,10 @@
         <v>0</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="R25" s="1" t="n">
         <v>3</v>
@@ -8523,21 +8522,21 @@
         <v>0</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AC25" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="AE25" s="0" t="s">
+      <c r="AC25" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="AI25" s="0" t="s">
+      <c r="AE25" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AI25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ25" s="0" t="s">
+      <c r="AJ25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AK25" s="1" t="b">
@@ -8548,12 +8547,12 @@
         <v>71</v>
       </c>
       <c r="AM25" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>31</v>
@@ -8574,10 +8573,10 @@
         <v>0</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>31</v>
@@ -8598,10 +8597,10 @@
         <v>2816</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="R26" s="1" t="n">
         <v>4</v>
@@ -8629,21 +8628,21 @@
         <v>0</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AB26" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="AC26" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="AI26" s="0" t="s">
+      <c r="AC26" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ26" s="0" t="s">
+      <c r="AJ26" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AK26" s="1" t="b">
@@ -8654,12 +8653,12 @@
         <v>71</v>
       </c>
       <c r="AM26" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="159.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>31</v>
@@ -8680,10 +8679,10 @@
         <v>3968</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>31</v>
@@ -8704,10 +8703,10 @@
         <v>4736</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="R27" s="1" t="n">
         <v>10</v>
@@ -8735,19 +8734,19 @@
         <v>0</v>
       </c>
       <c r="Z27" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AH27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI27" s="0" t="s">
+      <c r="AI27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ27" s="0" t="s">
-        <v>253</v>
+      <c r="AJ27" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="AK27" s="1" t="b">
         <f aca="false">FALSE()</f>
@@ -8757,12 +8756,12 @@
         <v>71</v>
       </c>
       <c r="AM27" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>31</v>
@@ -8783,10 +8782,10 @@
         <v>0</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>31</v>
@@ -8807,10 +8806,10 @@
         <v>4608</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="R28" s="1" t="n">
         <v>10</v>
@@ -8838,18 +8837,18 @@
         <v>1</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AH28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI28" s="0" t="s">
+      <c r="AI28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ28" s="0" t="s">
+      <c r="AJ28" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AK28" s="1" t="b">
@@ -8860,12 +8859,12 @@
         <v>71</v>
       </c>
       <c r="AM28" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>31</v>
@@ -8886,10 +8885,10 @@
         <v>5120</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>31</v>
@@ -8910,10 +8909,10 @@
         <v>0</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="R29" s="1" t="n">
         <v>3</v>
@@ -8944,12 +8943,12 @@
         <v>169</v>
       </c>
       <c r="AA29" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="AI29" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="AI29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ29" s="0" t="s">
+      <c r="AJ29" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AK29" s="1" t="b">
@@ -8960,12 +8959,12 @@
         <v>71</v>
       </c>
       <c r="AM29" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>31</v>
@@ -8986,10 +8985,10 @@
         <v>5376</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>31</v>
@@ -9010,10 +9009,10 @@
         <v>4992</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="R30" s="1" t="n">
         <v>10</v>
@@ -9041,19 +9040,19 @@
         <v>1</v>
       </c>
       <c r="Z30" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AA30" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="AF30" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="AI30" s="0" t="s">
+      <c r="AF30" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ30" s="0" t="s">
-        <v>278</v>
+      <c r="AJ30" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK30" s="1" t="b">
         <f aca="false">FALSE()</f>
@@ -9063,12 +9062,12 @@
         <v>71</v>
       </c>
       <c r="AM30" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>31</v>
@@ -9089,10 +9088,10 @@
         <v>2176</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>31</v>
@@ -9113,10 +9112,10 @@
         <v>0</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="R31" s="1" t="n">
         <v>6</v>
@@ -9144,19 +9143,19 @@
         <v>0</v>
       </c>
       <c r="Z31" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AA31" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="AF31" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="AI31" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ31" s="0" t="s">
-        <v>278</v>
+      <c r="AJ31" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK31" s="1" t="b">
         <f aca="false">FALSE()</f>
@@ -9166,12 +9165,12 @@
         <v>71</v>
       </c>
       <c r="AM31" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
@@ -9192,10 +9191,10 @@
         <v>6144</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>31</v>
@@ -9216,10 +9215,10 @@
         <v>2688</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="R32" s="1" t="n">
         <v>3</v>
@@ -9247,19 +9246,19 @@
         <v>0</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF32" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="AI32" s="0" t="s">
+      <c r="AF32" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="AI32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ32" s="0" t="s">
-        <v>278</v>
+      <c r="AJ32" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK32" s="1" t="b">
         <f aca="false">TRUE()</f>
@@ -9269,12 +9268,12 @@
         <v>71</v>
       </c>
       <c r="AM32" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>31</v>
@@ -9295,10 +9294,10 @@
         <v>3072</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>31</v>
@@ -9319,10 +9318,10 @@
         <v>2688</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="R33" s="1" t="n">
         <v>10</v>
@@ -9350,19 +9349,19 @@
         <v>1</v>
       </c>
       <c r="Z33" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AA33" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="AG33" s="0" t="n">
+        <v>303</v>
+      </c>
+      <c r="AG33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AI33" s="0" t="s">
+      <c r="AI33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ33" s="0" t="s">
-        <v>278</v>
+      <c r="AJ33" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK33" s="1" t="b">
         <f aca="false">FALSE()</f>
@@ -9372,12 +9371,12 @@
         <v>71</v>
       </c>
       <c r="AM33" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>31</v>
@@ -9398,10 +9397,10 @@
         <v>3072</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>31</v>
@@ -9422,10 +9421,10 @@
         <v>2688</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="R34" s="1" t="n">
         <v>1</v>
@@ -9453,16 +9452,16 @@
         <v>0</v>
       </c>
       <c r="AA34" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="AF34" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="AI34" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="AF34" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="AI34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ34" s="0" t="s">
-        <v>278</v>
+      <c r="AJ34" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK34" s="1" t="b">
         <f aca="false">TRUE()</f>
@@ -9472,12 +9471,12 @@
         <v>71</v>
       </c>
       <c r="AM34" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>31</v>
@@ -9498,10 +9497,10 @@
         <v>7040</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>31</v>
@@ -9522,10 +9521,10 @@
         <v>2688</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="R35" s="1" t="n">
         <v>2</v>
@@ -9553,16 +9552,16 @@
         <v>0</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AA35" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="AI35" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="AI35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ35" s="0" t="s">
-        <v>278</v>
+      <c r="AJ35" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK35" s="1" t="b">
         <f aca="false">FALSE()</f>
@@ -9572,12 +9571,12 @@
         <v>71</v>
       </c>
       <c r="AM35" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>31</v>
@@ -9598,10 +9597,10 @@
         <v>3072</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>31</v>
@@ -9622,10 +9621,10 @@
         <v>0</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="R36" s="1" t="n">
         <v>10</v>
@@ -9653,16 +9652,16 @@
         <v>1</v>
       </c>
       <c r="Z36" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AA36" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="AI36" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="AI36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ36" s="0" t="s">
-        <v>278</v>
+      <c r="AJ36" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK36" s="1" t="b">
         <f aca="false">FALSE()</f>
@@ -9672,12 +9671,12 @@
         <v>71</v>
       </c>
       <c r="AM36" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>31</v>
@@ -9698,10 +9697,10 @@
         <v>0</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>31</v>
@@ -9722,10 +9721,10 @@
         <v>0</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="R37" s="1" t="n">
         <v>10</v>
@@ -9753,16 +9752,16 @@
         <v>1</v>
       </c>
       <c r="Z37" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AA37" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="AI37" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="AI37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ37" s="0" t="s">
-        <v>278</v>
+      <c r="AJ37" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="AK37" s="1" t="b">
         <f aca="false">FALSE()</f>
@@ -9772,7 +9771,7 @@
         <v>71</v>
       </c>
       <c r="AM37" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="108.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>